<commit_message>
Traspasado todo lo del RMD al RMW
Archivo PDF con todo lo escrito del trabajo hasta el momento
</commit_message>
<xml_diff>
--- a/Variables descripcion.xlsx
+++ b/Variables descripcion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Documents\GitHub\TFG-Baloncesto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Documents\GitHub\TFG-Baloncesto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC74F8CC-1138-4D7A-9B37-AD66D9108033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB579B54-E2B4-4B48-925A-3F4DDCA93FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{A61D08D2-FFC3-49B9-870A-D1CDB3FBC47C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>2FGM</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>Tapon recibido</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,6 +756,9 @@
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">

</xml_diff>